<commit_message>
Actualización del archivo de registros con nuevos datos
</commit_message>
<xml_diff>
--- a/registro_usuarios.xlsx
+++ b/registro_usuarios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -791,6 +791,300 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>65</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>130</v>
+      </c>
+      <c r="R4" t="n">
+        <v>85</v>
+      </c>
+      <c r="S4" t="n">
+        <v>190</v>
+      </c>
+      <c r="T4" t="n">
+        <v>110</v>
+      </c>
+      <c r="U4" t="n">
+        <v>50</v>
+      </c>
+      <c r="V4" t="n">
+        <v>150</v>
+      </c>
+      <c r="W4" t="n">
+        <v>27</v>
+      </c>
+      <c r="X4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>65</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>130</v>
+      </c>
+      <c r="R5" t="n">
+        <v>85</v>
+      </c>
+      <c r="S5" t="n">
+        <v>190</v>
+      </c>
+      <c r="T5" t="n">
+        <v>110</v>
+      </c>
+      <c r="U5" t="n">
+        <v>50</v>
+      </c>
+      <c r="V5" t="n">
+        <v>150</v>
+      </c>
+      <c r="W5" t="n">
+        <v>27</v>
+      </c>
+      <c r="X5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>65</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>130</v>
+      </c>
+      <c r="R6" t="n">
+        <v>85</v>
+      </c>
+      <c r="S6" t="n">
+        <v>190</v>
+      </c>
+      <c r="T6" t="n">
+        <v>110</v>
+      </c>
+      <c r="U6" t="n">
+        <v>50</v>
+      </c>
+      <c r="V6" t="n">
+        <v>150</v>
+      </c>
+      <c r="W6" t="n">
+        <v>27</v>
+      </c>
+      <c r="X6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>